<commit_message>
Added script and white noise data
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pooyan/Repos/uncertainty/data/cassandra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pjamshidi/devrepo/uncertainty1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="max-min" sheetId="1" r:id="rId1"/>
     <sheet name="rank" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -187,6 +187,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -454,7 +457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -701,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,92 +716,123 @@
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B2">
         <v>3.6400000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>-7.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B3">
         <v>-0.17319999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>-5.2699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4">
         <v>3.1800000000000002E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>6.9599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5">
         <v>8.8000000000000005E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1.3899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B6">
         <v>-7.0400000000000004E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>3.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B7">
         <v>2.1700000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B8">
         <v>-0.12659999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B9">
         <v>0.1424</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>7.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B10">
         <v>0.10009999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>-3.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B11">
         <v>-3.27E-2</v>
       </c>
+      <c r="C11">
+        <v>1.9199999999999998E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>